<commit_message>
update new train data
</commit_message>
<xml_diff>
--- a/rossmann/rossmann.xlsx
+++ b/rossmann/rossmann.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="134">
   <si>
     <t xml:space="preserve">store </t>
     <phoneticPr fontId="4"/>
@@ -746,6 +746,14 @@
     <t>score</t>
     <phoneticPr fontId="4"/>
   </si>
+  <si>
+    <t>train+store+weather+avg_sales</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>train_20151109_1</t>
+    <phoneticPr fontId="4"/>
+  </si>
 </sst>
 </file>
 
@@ -3591,11 +3599,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2093340856"/>
-        <c:axId val="2093343192"/>
+        <c:axId val="2117428616"/>
+        <c:axId val="2117376680"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2093340856"/>
+        <c:axId val="2117428616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3604,7 +3612,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2093343192"/>
+        <c:crossAx val="2117376680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3612,7 +3620,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2093343192"/>
+        <c:axId val="2117376680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3623,7 +3631,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2093340856"/>
+        <c:crossAx val="2117428616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6510,11 +6518,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2093351576"/>
-        <c:axId val="2093354568"/>
+        <c:axId val="2116056200"/>
+        <c:axId val="2116033928"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2093351576"/>
+        <c:axId val="2116056200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6523,7 +6531,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2093354568"/>
+        <c:crossAx val="2116033928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6531,7 +6539,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2093354568"/>
+        <c:axId val="2116033928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6542,7 +6550,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2093351576"/>
+        <c:crossAx val="2116056200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7957,16 +7965,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:Z5"/>
+  <dimension ref="B3:Z6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="23.5" customWidth="1"/>
+    <col min="3" max="3" width="33.1640625" customWidth="1"/>
+    <col min="4" max="5" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:26">
@@ -8115,6 +8124,17 @@
       </c>
       <c r="Z5" t="s">
         <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="2:26">
+      <c r="B6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6">
+        <v>412540.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
train + weather + avg
</commit_message>
<xml_diff>
--- a/rossmann/rossmann.xlsx
+++ b/rossmann/rossmann.xlsx
@@ -3599,11 +3599,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2117428616"/>
-        <c:axId val="2117376680"/>
+        <c:axId val="2109064888"/>
+        <c:axId val="2109067624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2117428616"/>
+        <c:axId val="2109064888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3612,7 +3612,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117376680"/>
+        <c:crossAx val="2109067624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3620,7 +3620,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2117376680"/>
+        <c:axId val="2109067624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3631,7 +3631,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117428616"/>
+        <c:crossAx val="2109064888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6518,11 +6518,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2116056200"/>
-        <c:axId val="2116033928"/>
+        <c:axId val="2109466664"/>
+        <c:axId val="2109469608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2116056200"/>
+        <c:axId val="2109466664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6531,7 +6531,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116033928"/>
+        <c:crossAx val="2109469608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6539,7 +6539,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2116033928"/>
+        <c:axId val="2109469608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6550,7 +6550,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116056200"/>
+        <c:crossAx val="2109466664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7968,7 +7968,7 @@
   <dimension ref="B3:Z6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -8135,6 +8135,9 @@
       </c>
       <c r="D6">
         <v>412540.1</v>
+      </c>
+      <c r="E6">
+        <v>0.16286999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>